<commit_message>
tela de login inicial
</commit_message>
<xml_diff>
--- a/Documentação/backlog_omniview.xlsx
+++ b/Documentação/backlog_omniview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\Grupo-7\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupolinx-my.sharepoint.com/personal/mariana_cazzoto_linx_com_br/Documents/Documentos/Grupo-7/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4812C772-C435-4BA0-B806-97E36EC5A555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="525" windowWidth="19905" windowHeight="11505" xr2:uid="{5EBC7968-C925-4080-A562-A43DF5B640B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5EBC7968-C925-4080-A562-A43DF5B640B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -683,45 +682,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -737,29 +700,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -795,6 +740,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +874,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1177,106 +1176,106 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="100.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="100.26953125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="10"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="10"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="36"/>
-    </row>
-    <row r="6" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1285,18 +1284,18 @@
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
-    </row>
-    <row r="7" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1308,15 +1307,15 @@
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1328,35 +1327,35 @@
       <c r="D8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1368,15 +1367,15 @@
       <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="F10" s="18"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1388,15 +1387,15 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="37"/>
-    </row>
-    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1408,35 +1407,35 @@
       <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="37"/>
-    </row>
-    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="F12" s="18"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="37"/>
-    </row>
-    <row r="14" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1448,15 +1447,15 @@
       <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="F14" s="18"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1468,15 +1467,15 @@
       <c r="D15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1488,15 +1487,15 @@
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="43"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1508,35 +1507,35 @@
       <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+      <c r="F17" s="25"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="37"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="s">
+      <c r="F18" s="25"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="5">
@@ -1548,46 +1547,46 @@
       <c r="D19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="F19" s="29"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="37" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="20" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A1:D3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="E1:G3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A1:D3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>